<commit_message>
Added backend API Risk
</commit_message>
<xml_diff>
--- a/PMIS/RIC Register.xlsx
+++ b/PMIS/RIC Register.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\OneDrive\Documents\Uni\Year 3\Group Project\PMIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\OneDrive\Documents\Uni\Year 3\Group Project\PMIS\Live Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{36A3240F-55D0-4AB7-832A-C00AF8DB2E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4B6E15FE-4A2F-4F20-BB86-DFC1DF68C223}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{36A3240F-55D0-4AB7-832A-C00AF8DB2E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02C86509-EF19-4CBE-9FF1-52C2C5A30B47}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Away team member will do their best to complete assigned work and will collaborate with other team members to work around this.</t>
+  </si>
+  <si>
+    <t>Nuvven does not have all backend components ready, slowing down the teams progress. This may also increase the expected workload of the team.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Additional work will be deflected as team does not have time to finish assigned work and complete backend API work.</t>
   </si>
 </sst>
 </file>
@@ -584,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="79" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="79" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,8 +1096,11 @@
       <c r="I16" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J16" s="8">
+        <v>43888</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1016</v>
       </c>
@@ -1118,7 +1130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1017</v>
       </c>
@@ -1147,86 +1159,113 @@
       <c r="I18" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="9" t="str">
+      <c r="J18" s="8">
+        <v>43892</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>1018</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="8">
+        <v>43897</v>
+      </c>
+      <c r="E19" s="7">
+        <v>70</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45.5</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G21" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G23" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G24" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G25" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G26" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G27" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G28" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G29" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G30" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G31" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G32" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
Added Covid 19 risk
</commit_message>
<xml_diff>
--- a/PMIS/RIC Register.xlsx
+++ b/PMIS/RIC Register.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\OneDrive\Documents\Uni\Year 3\Group Project\PMIS\Live Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ca01c0acc71d382/Documents/Uni/Year 3/Group Project/PMIS/Live Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{36A3240F-55D0-4AB7-832A-C00AF8DB2E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02C86509-EF19-4CBE-9FF1-52C2C5A30B47}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{36A3240F-55D0-4AB7-832A-C00AF8DB2E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8470E81B-1124-4D1A-B678-89FF0C592378}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Additional work will be deflected as team does not have time to finish assigned work and complete backend API work.</t>
+  </si>
+  <si>
+    <t>With the increased risk from Covid 19, team members are more likely to get sick and be unable to work.</t>
+  </si>
+  <si>
+    <t>Team members will take all appropriate measures to stay healthy, including proper handwashing and self-isolation.</t>
   </si>
 </sst>
 </file>
@@ -594,7 +600,7 @@
   <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="79" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,6 +1042,9 @@
       <c r="I14" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="J14" s="8">
+        <v>43915</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -1193,10 +1202,34 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="9" t="str">
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>1019</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8">
+        <v>43913</v>
+      </c>
+      <c r="E20" s="7">
+        <v>50</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="9">
         <f t="shared" si="0"/>
-        <v/>
+        <v>25</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>